<commit_message>
Added Documentation for UART and Unit Tests
</commit_message>
<xml_diff>
--- a/PCB_POPULATION/RemoteLabs_supervisor_PCBV1.2.xlsx
+++ b/PCB_POPULATION/RemoteLabs_supervisor_PCBV1.2.xlsx
@@ -673,7 +673,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -804,13 +804,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1166,13 +1159,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1180,12 +1172,11 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1511,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1527,30 +1518,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1">
@@ -1570,7 +1561,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1">
@@ -1590,7 +1581,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1">
@@ -1610,7 +1601,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="1">
@@ -1629,11 +1620,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="5"/>
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+      <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="1">
@@ -1653,7 +1644,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="1">
@@ -1673,7 +1664,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+      <c r="A9" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="1">
@@ -1693,7 +1684,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="A10" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="1">
@@ -1713,7 +1704,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="1">
@@ -1733,7 +1724,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
+      <c r="A12" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="1">
@@ -1753,7 +1744,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="1">
@@ -1773,7 +1764,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="1">
@@ -1793,7 +1784,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="9" t="s">
+      <c r="A15" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="1">
@@ -1812,8 +1803,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="5"/>
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
@@ -1836,7 +1827,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>47</v>
       </c>
       <c r="B18" s="1">
@@ -1856,7 +1847,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
+      <c r="A19" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="1">
@@ -1876,7 +1867,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+      <c r="A20" t="s">
         <v>56</v>
       </c>
       <c r="B20" s="1">
@@ -1896,7 +1887,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>61</v>
       </c>
       <c r="B21" s="1">
@@ -1916,7 +1907,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="9" t="s">
+      <c r="A22" t="s">
         <v>63</v>
       </c>
       <c r="B22" s="1">
@@ -1935,11 +1926,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="4" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="5"/>
+    <row r="23" spans="1:6" s="3" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B24" s="1">
@@ -1959,7 +1950,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B25" s="1">
@@ -1978,12 +1969,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="4" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="6"/>
-      <c r="B26" s="5"/>
+    <row r="26" spans="1:6" s="3" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="5"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+      <c r="A27" t="s">
         <v>70</v>
       </c>
       <c r="B27" s="1">
@@ -2003,7 +1994,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="3" t="s">
+      <c r="A28" t="s">
         <v>74</v>
       </c>
       <c r="B28" s="1">
@@ -2022,11 +2013,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="5"/>
+    <row r="29" spans="1:6" s="3" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="9" t="s">
+      <c r="A30" t="s">
         <v>76</v>
       </c>
       <c r="B30" s="1">
@@ -2045,11 +2036,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="5"/>
+    <row r="31" spans="1:6" s="3" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
+      <c r="A32" t="s">
         <v>81</v>
       </c>
       <c r="B32" s="1">
@@ -2069,7 +2060,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+      <c r="A33" t="s">
         <v>86</v>
       </c>
       <c r="B33" s="1">
@@ -2089,7 +2080,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="A34" t="s">
         <v>91</v>
       </c>
       <c r="B34" s="1">
@@ -2109,7 +2100,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
+      <c r="A35" t="s">
         <v>95</v>
       </c>
       <c r="B35" s="1">
@@ -2129,7 +2120,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+      <c r="A36" t="s">
         <v>99</v>
       </c>
       <c r="B36" s="1">
@@ -2149,7 +2140,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
+      <c r="A37" t="s">
         <v>103</v>
       </c>
       <c r="B37" s="1">
@@ -2169,7 +2160,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="9" t="s">
+      <c r="A38" t="s">
         <v>108</v>
       </c>
       <c r="B38" s="1">
@@ -2189,7 +2180,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+      <c r="A39" t="s">
         <v>112</v>
       </c>
       <c r="B39" s="1">
@@ -2209,7 +2200,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="3" t="s">
+      <c r="A40" t="s">
         <v>114</v>
       </c>
       <c r="B40" s="1">
@@ -2229,7 +2220,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
+      <c r="A41" t="s">
         <v>119</v>
       </c>
       <c r="B41" s="1">
@@ -2249,7 +2240,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
+      <c r="A42" t="s">
         <v>121</v>
       </c>
       <c r="B42" s="1">
@@ -2269,7 +2260,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="s">
+      <c r="A43" t="s">
         <v>126</v>
       </c>
       <c r="B43" s="1">
@@ -2289,7 +2280,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
+      <c r="A44" t="s">
         <v>130</v>
       </c>
       <c r="B44" s="1">
@@ -2309,7 +2300,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
+      <c r="A45" t="s">
         <v>132</v>
       </c>
       <c r="B45" s="1">
@@ -2329,7 +2320,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="s">
+      <c r="A46" t="s">
         <v>134</v>
       </c>
       <c r="B46" s="1">
@@ -2349,7 +2340,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="s">
+      <c r="A47" t="s">
         <v>136</v>
       </c>
       <c r="B47" s="1">
@@ -2369,7 +2360,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="s">
+      <c r="A48" t="s">
         <v>138</v>
       </c>
       <c r="B48" s="1">
@@ -2389,7 +2380,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
+      <c r="A49" t="s">
         <v>140</v>
       </c>
       <c r="B49" s="1">
@@ -2409,7 +2400,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="3" t="s">
+      <c r="A50" t="s">
         <v>142</v>
       </c>
       <c r="B50" s="1">
@@ -2428,11 +2419,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="4" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="5"/>
+    <row r="51" spans="1:6" s="3" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="3" t="s">
+      <c r="A52" t="s">
         <v>144</v>
       </c>
       <c r="B52" s="1">
@@ -2451,11 +2442,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="4" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="5"/>
+    <row r="53" spans="1:6" s="3" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="9" t="s">
+      <c r="A54" t="s">
         <v>148</v>
       </c>
       <c r="B54" s="1">
@@ -2475,7 +2466,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="8" t="s">
         <v>153</v>
       </c>
       <c r="B55" s="1">
@@ -2495,7 +2486,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="9" t="s">
+      <c r="A56" t="s">
         <v>155</v>
       </c>
       <c r="B56" s="1">
@@ -2515,7 +2506,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="8" t="s">
         <v>157</v>
       </c>
       <c r="B57" s="1">
@@ -2535,7 +2526,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="9" t="s">
+      <c r="A58" t="s">
         <v>159</v>
       </c>
       <c r="B58" s="1">
@@ -2555,7 +2546,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="8" t="s">
         <v>161</v>
       </c>
       <c r="B59" s="1">
@@ -2575,7 +2566,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="9" t="s">
+      <c r="A60" t="s">
         <v>163</v>
       </c>
       <c r="B60" s="1">
@@ -2594,8 +2585,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="4" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="5"/>
+    <row r="61" spans="1:6" s="3" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
@@ -2618,7 +2609,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="9" t="s">
+      <c r="A63" t="s">
         <v>170</v>
       </c>
       <c r="B63" s="1">
@@ -2638,7 +2629,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="9" t="s">
+      <c r="A64" t="s">
         <v>175</v>
       </c>
       <c r="B64" s="1">
@@ -2657,11 +2648,11 @@
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="4" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B65" s="5"/>
+    <row r="65" spans="1:6" s="3" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="3" t="s">
+      <c r="A66" t="s">
         <v>177</v>
       </c>
       <c r="B66" s="1">
@@ -2681,7 +2672,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="9" t="s">
+      <c r="A67" t="s">
         <v>181</v>
       </c>
       <c r="B67" s="1">
@@ -2721,7 +2712,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="9" t="s">
+      <c r="A69" t="s">
         <v>189</v>
       </c>
       <c r="B69" s="1">
@@ -2741,7 +2732,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="9" t="s">
+      <c r="A70" t="s">
         <v>192</v>
       </c>
       <c r="B70" s="1">
@@ -2761,7 +2752,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="9" t="s">
+      <c r="A71" t="s">
         <v>196</v>
       </c>
       <c r="B71" s="1">
@@ -2781,7 +2772,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="9" t="s">
+      <c r="A72" t="s">
         <v>199</v>
       </c>
       <c r="B72" s="1">
@@ -2801,7 +2792,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="9" t="s">
+      <c r="A73" t="s">
         <v>203</v>
       </c>
       <c r="B73" s="1">
@@ -2821,7 +2812,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="9" t="s">
+      <c r="A74" t="s">
         <v>206</v>
       </c>
       <c r="B74" s="1">
@@ -2840,11 +2831,11 @@
         <v>208</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="4" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B75" s="5"/>
+    <row r="75" spans="1:6" s="3" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B75" s="4"/>
     </row>
     <row r="76" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="9" t="s">
+      <c r="A76" t="s">
         <v>209</v>
       </c>
       <c r="B76" s="1">

</xml_diff>